<commit_message>
library yield ng and enrichment kit - optional
</commit_message>
<xml_diff>
--- a/template_examples/rna_bam_template.xlsx
+++ b/template_examples/rna_bam_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500F321A-93ED-BE4B-BE1B-49BDE2E10DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A88818C-DFC9-6A44-986E-3255545C7C18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="1120" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RNA" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="69">
   <si>
     <t>#t</t>
   </si>
@@ -881,7 +881,7 @@
   <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -952,16 +952,14 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1070,9 +1068,6 @@
       <c r="C12" t="s">
         <v>66</v>
       </c>
-      <c r="D12">
-        <v>650</v>
-      </c>
       <c r="E12">
         <v>0.8</v>
       </c>
@@ -2081,7 +2076,7 @@
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B9:H9"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="5">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{6AC1EC70-19F6-E146-BE12-67BC1C6823E1}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>

</xml_diff>